<commit_message>
created database on base model and created services for the db instead of excel via dependency injection.
</commit_message>
<xml_diff>
--- a/EskitechApi/Data/skistore_produkter.xlsx
+++ b/EskitechApi/Data/skistore_produkter.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="14055" windowHeight="11835"/>
+    <workbookView windowWidth="28380" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1064,8 +1064,8 @@
   <sheetPr/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>

</xml_diff>